<commit_message>
Random_forest sans missing values
</commit_message>
<xml_diff>
--- a/machine_learning/Test_result_Annab.xlsx
+++ b/machine_learning/Test_result_Annab.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG98"/>
+  <dimension ref="A1:AC98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,26 +576,6 @@
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>bug type</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>species</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>bug_category</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
           <t>predicted_bug_category</t>
         </is>
       </c>
@@ -687,26 +667,6 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -798,26 +758,6 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -909,26 +849,6 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -1020,26 +940,6 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -1131,26 +1031,6 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -1242,26 +1122,6 @@
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -1353,26 +1213,6 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -1464,26 +1304,6 @@
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF9" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -1575,26 +1395,6 @@
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -1686,26 +1486,6 @@
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE11" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF11" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG11" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -1797,26 +1577,6 @@
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD12" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE12" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF12" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG12" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -1908,26 +1668,6 @@
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF13" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG13" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -2019,26 +1759,6 @@
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD14" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE14" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF14" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG14" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -2130,26 +1850,6 @@
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD15" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE15" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF15" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG15" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -2241,26 +1941,6 @@
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD16" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE16" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF16" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG16" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -2352,26 +2032,6 @@
       </c>
       <c r="AC17" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE17" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF17" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG17" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -2463,26 +2123,6 @@
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD18" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF18" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG18" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -2574,26 +2214,6 @@
       </c>
       <c r="AC19" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD19" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF19" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG19" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -2685,26 +2305,6 @@
       </c>
       <c r="AC20" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD20" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE20" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF20" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG20" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -2796,26 +2396,6 @@
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD21" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE21" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF21" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG21" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -2907,26 +2487,6 @@
       </c>
       <c r="AC22" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD22" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE22" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF22" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG22" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3018,26 +2578,6 @@
       </c>
       <c r="AC23" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD23" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE23" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF23" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG23" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3129,26 +2669,6 @@
       </c>
       <c r="AC24" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD24" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE24" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF24" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG24" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3240,26 +2760,6 @@
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD25" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE25" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF25" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG25" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3351,26 +2851,6 @@
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD26" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE26" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF26" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG26" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3462,26 +2942,6 @@
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD27" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE27" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF27" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG27" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3573,26 +3033,6 @@
       </c>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD28" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE28" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF28" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG28" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3684,26 +3124,6 @@
       </c>
       <c r="AC29" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD29" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE29" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF29" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG29" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3795,26 +3215,6 @@
       </c>
       <c r="AC30" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD30" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE30" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF30" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG30" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -3906,26 +3306,6 @@
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD31" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE31" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF31" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG31" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4017,26 +3397,6 @@
       </c>
       <c r="AC32" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD32" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE32" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF32" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG32" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4128,26 +3488,6 @@
       </c>
       <c r="AC33" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD33" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE33" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF33" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG33" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4239,26 +3579,6 @@
       </c>
       <c r="AC34" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD34" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE34" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF34" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG34" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4350,26 +3670,6 @@
       </c>
       <c r="AC35" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD35" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE35" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF35" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG35" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4461,26 +3761,6 @@
       </c>
       <c r="AC36" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD36" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE36" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF36" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG36" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4572,26 +3852,6 @@
       </c>
       <c r="AC37" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD37" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE37" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF37" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG37" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4683,26 +3943,6 @@
       </c>
       <c r="AC38" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD38" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE38" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF38" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG38" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4794,26 +4034,6 @@
       </c>
       <c r="AC39" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD39" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE39" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF39" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG39" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -4905,26 +4125,6 @@
       </c>
       <c r="AC40" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD40" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE40" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF40" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG40" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5016,26 +4216,6 @@
       </c>
       <c r="AC41" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD41" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE41" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF41" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG41" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5127,26 +4307,6 @@
       </c>
       <c r="AC42" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD42" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE42" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF42" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG42" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5238,26 +4398,6 @@
       </c>
       <c r="AC43" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD43" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE43" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF43" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG43" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5349,26 +4489,6 @@
       </c>
       <c r="AC44" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD44" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE44" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF44" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG44" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5460,26 +4580,6 @@
       </c>
       <c r="AC45" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD45" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE45" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF45" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG45" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5571,26 +4671,6 @@
       </c>
       <c r="AC46" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD46" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE46" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF46" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG46" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5682,26 +4762,6 @@
       </c>
       <c r="AC47" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD47" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE47" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF47" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG47" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -5793,26 +4853,6 @@
       </c>
       <c r="AC48" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD48" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE48" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF48" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG48" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -5904,26 +4944,6 @@
       </c>
       <c r="AC49" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD49" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE49" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF49" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG49" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6015,26 +5035,6 @@
       </c>
       <c r="AC50" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD50" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE50" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF50" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG50" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6126,26 +5126,6 @@
       </c>
       <c r="AC51" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD51" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE51" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF51" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG51" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6237,26 +5217,6 @@
       </c>
       <c r="AC52" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD52" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE52" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF52" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG52" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6348,26 +5308,6 @@
       </c>
       <c r="AC53" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD53" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE53" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF53" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG53" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6459,26 +5399,6 @@
       </c>
       <c r="AC54" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD54" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE54" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF54" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG54" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6570,26 +5490,6 @@
       </c>
       <c r="AC55" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD55" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE55" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF55" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG55" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6681,26 +5581,6 @@
       </c>
       <c r="AC56" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD56" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE56" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF56" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG56" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -6792,26 +5672,6 @@
       </c>
       <c r="AC57" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD57" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE57" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF57" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG57" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -6903,26 +5763,6 @@
       </c>
       <c r="AC58" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD58" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE58" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF58" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG58" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -7014,26 +5854,6 @@
       </c>
       <c r="AC59" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD59" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE59" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF59" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG59" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -7124,26 +5944,6 @@
         <v>25.38462644795755</v>
       </c>
       <c r="AC60" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD60" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE60" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF60" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG60" t="inlineStr">
         <is>
           <t>Bee</t>
         </is>
@@ -7236,26 +6036,6 @@
       </c>
       <c r="AC61" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD61" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE61" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF61" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG61" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -7347,26 +6127,6 @@
       </c>
       <c r="AC62" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD62" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE62" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF62" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG62" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -7458,26 +6218,6 @@
       </c>
       <c r="AC63" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD63" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE63" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF63" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG63" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -7569,26 +6309,6 @@
       </c>
       <c r="AC64" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD64" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE64" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF64" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG64" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -7680,26 +6400,6 @@
       </c>
       <c r="AC65" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD65" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE65" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF65" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG65" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -7791,26 +6491,6 @@
       </c>
       <c r="AC66" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD66" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE66" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF66" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG66" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -7902,26 +6582,6 @@
       </c>
       <c r="AC67" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD67" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE67" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF67" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG67" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -8013,26 +6673,6 @@
       </c>
       <c r="AC68" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD68" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE68" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF68" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG68" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -8124,26 +6764,6 @@
       </c>
       <c r="AC69" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD69" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE69" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF69" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG69" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -8235,26 +6855,6 @@
       </c>
       <c r="AC70" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD70" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE70" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF70" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG70" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -8346,26 +6946,6 @@
       </c>
       <c r="AC71" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD71" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE71" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF71" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG71" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -8457,26 +7037,6 @@
       </c>
       <c r="AC72" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD72" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE72" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF72" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG72" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -8568,26 +7128,6 @@
       </c>
       <c r="AC73" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD73" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE73" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF73" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG73" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -8679,26 +7219,6 @@
       </c>
       <c r="AC74" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD74" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE74" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF74" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG74" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -8790,26 +7310,6 @@
       </c>
       <c r="AC75" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD75" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE75" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF75" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG75" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -8901,26 +7401,6 @@
       </c>
       <c r="AC76" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD76" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE76" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF76" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG76" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -9012,26 +7492,6 @@
       </c>
       <c r="AC77" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD77" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE77" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF77" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG77" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -9123,26 +7583,6 @@
       </c>
       <c r="AC78" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD78" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE78" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF78" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG78" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -9234,26 +7674,6 @@
       </c>
       <c r="AC79" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD79" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE79" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF79" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG79" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -9345,26 +7765,6 @@
       </c>
       <c r="AC80" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD80" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE80" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF80" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG80" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -9456,26 +7856,6 @@
       </c>
       <c r="AC81" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD81" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE81" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF81" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG81" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -9567,26 +7947,6 @@
       </c>
       <c r="AC82" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD82" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE82" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF82" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG82" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -9678,26 +8038,6 @@
       </c>
       <c r="AC83" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD83" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE83" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF83" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG83" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -9789,26 +8129,6 @@
       </c>
       <c r="AC84" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD84" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE84" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF84" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG84" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -9900,26 +8220,6 @@
       </c>
       <c r="AC85" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD85" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE85" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF85" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG85" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10011,26 +8311,6 @@
       </c>
       <c r="AC86" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD86" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE86" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF86" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG86" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10122,26 +8402,6 @@
       </c>
       <c r="AC87" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD87" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE87" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF87" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG87" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -10233,26 +8493,6 @@
       </c>
       <c r="AC88" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD88" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE88" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF88" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG88" t="inlineStr">
-        <is>
           <t>Bumblebee</t>
         </is>
       </c>
@@ -10344,26 +8584,6 @@
       </c>
       <c r="AC89" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD89" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE89" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF89" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG89" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10455,26 +8675,6 @@
       </c>
       <c r="AC90" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD90" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE90" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF90" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG90" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10566,26 +8766,6 @@
       </c>
       <c r="AC91" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD91" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE91" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF91" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG91" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10677,26 +8857,6 @@
       </c>
       <c r="AC92" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD92" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE92" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF92" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG92" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10788,26 +8948,6 @@
       </c>
       <c r="AC93" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD93" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE93" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF93" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG93" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -10899,26 +9039,6 @@
       </c>
       <c r="AC94" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD94" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE94" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF94" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG94" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -11010,26 +9130,6 @@
       </c>
       <c r="AC95" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD95" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE95" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF95" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG95" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -11121,26 +9221,6 @@
       </c>
       <c r="AC96" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD96" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE96" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF96" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG96" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -11232,26 +9312,6 @@
       </c>
       <c r="AC97" t="inlineStr">
         <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD97" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE97" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF97" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG97" t="inlineStr">
-        <is>
           <t>Bee</t>
         </is>
       </c>
@@ -11342,26 +9402,6 @@
         <v>32.62646278623244</v>
       </c>
       <c r="AC98" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AD98" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AE98" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AF98" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-      <c r="AG98" t="inlineStr">
         <is>
           <t>Bee</t>
         </is>

</xml_diff>